<commit_message>
dashboard, filter by status_akhir, notifikasi
</commit_message>
<xml_diff>
--- a/storage/import/barang.xlsx
+++ b/storage/import/barang.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS-A4\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS-A4\Documents\SUMO\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7635"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12315"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="822" uniqueCount="286">
   <si>
     <t>nama_barang</t>
   </si>
@@ -45,9 +45,6 @@
     <t>ATK</t>
   </si>
   <si>
-    <t>BUAH</t>
-  </si>
-  <si>
     <t>AMPLOP COKLAT TANPA TALI</t>
   </si>
   <si>
@@ -336,24 +333,576 @@
     <t>TISSUE</t>
   </si>
   <si>
-    <t>LAPTOP</t>
-  </si>
-  <si>
-    <t>Asus XT1T</t>
-  </si>
-  <si>
     <t>ASSET/NONASSET</t>
+  </si>
+  <si>
+    <t>KURSI AMAZY INFORMA</t>
+  </si>
+  <si>
+    <t>KURSI MANAGER</t>
+  </si>
+  <si>
+    <t>KURSI TINGGI</t>
+  </si>
+  <si>
+    <t>LEMARI FILE BESI</t>
+  </si>
+  <si>
+    <t>MEJA ADMIN PANEL</t>
+  </si>
+  <si>
+    <t>MEJA AMAZY KECIL</t>
+  </si>
+  <si>
+    <t>UNIT</t>
+  </si>
+  <si>
+    <t>APAR PYRAMID</t>
+  </si>
+  <si>
+    <t>BEAN BAG</t>
+  </si>
+  <si>
+    <t>BLOWER TANGAN RYU</t>
+  </si>
+  <si>
+    <t>CERMIN</t>
+  </si>
+  <si>
+    <t>FILE KABINET PANEL</t>
+  </si>
+  <si>
+    <t>FLY TRAP</t>
+  </si>
+  <si>
+    <t>GIMBAL KAMERA</t>
+  </si>
+  <si>
+    <t>HEADLAMP SENTER</t>
+  </si>
+  <si>
+    <t>HOT AIR GUN SELLERY</t>
+  </si>
+  <si>
+    <t>INFOCUS</t>
+  </si>
+  <si>
+    <t>KAMERA CANON</t>
+  </si>
+  <si>
+    <t>KARPET MUSHOLLA</t>
+  </si>
+  <si>
+    <t>KITCHEN SET ALUMUNIUM</t>
+  </si>
+  <si>
+    <t>KITCHEN SET MULTIPLEK</t>
+  </si>
+  <si>
+    <t>KURSI ALUMUNIUM</t>
+  </si>
+  <si>
+    <t>KURSI BAR</t>
+  </si>
+  <si>
+    <t>KURSI BROTHER BIRU</t>
+  </si>
+  <si>
+    <t>KURSI BASO</t>
+  </si>
+  <si>
+    <t>KURSI KULIAH</t>
+  </si>
+  <si>
+    <t>KURSI PUTAR</t>
+  </si>
+  <si>
+    <t>KURSI TAMU</t>
+  </si>
+  <si>
+    <t>KURSI TUNGGU BESI INFORMA</t>
+  </si>
+  <si>
+    <t>LACI FILE KABINET</t>
+  </si>
+  <si>
+    <t>LEMARI BERKAS KAYU</t>
+  </si>
+  <si>
+    <t>LEMARI DINDING</t>
+  </si>
+  <si>
+    <t>LEMARI FILE</t>
+  </si>
+  <si>
+    <t>LEMARI KACA</t>
+  </si>
+  <si>
+    <t>LEMARI LOKER</t>
+  </si>
+  <si>
+    <t>LEMARI LOKER BESI</t>
+  </si>
+  <si>
+    <t>LEMARI PANEL</t>
+  </si>
+  <si>
+    <t>LEMARI PLASTIK</t>
+  </si>
+  <si>
+    <t>LIGHTING</t>
+  </si>
+  <si>
+    <t>MEJA AMAZY BESAR</t>
+  </si>
+  <si>
+    <t>MEJA BUNDAR KACA INFORMA</t>
+  </si>
+  <si>
+    <t>MEJA KANTIN KECIL</t>
+  </si>
+  <si>
+    <t>MEJA MANAGER</t>
+  </si>
+  <si>
+    <t>MEJA OVAL</t>
+  </si>
+  <si>
+    <t>MEJA PELAYANAN</t>
+  </si>
+  <si>
+    <t>MEJA TAMU KACA</t>
+  </si>
+  <si>
+    <t>MEJA WORKSTATION</t>
+  </si>
+  <si>
+    <t>MESIN HITUNG UANG KRISBOW</t>
+  </si>
+  <si>
+    <t>MESIN LAMINASI</t>
+  </si>
+  <si>
+    <t>MESIN WRAPING WIRAPAX</t>
+  </si>
+  <si>
+    <t>PAPAN FLIPCHART</t>
+  </si>
+  <si>
+    <t>PAPAN TULIS</t>
+  </si>
+  <si>
+    <t>RAK AMBALAN</t>
+  </si>
+  <si>
+    <t>RAK SIKU</t>
+  </si>
+  <si>
+    <t>RAK DINDING</t>
+  </si>
+  <si>
+    <t>RAK BUKU</t>
+  </si>
+  <si>
+    <t>SET MEJA KURSI ROTAN KOTAK</t>
+  </si>
+  <si>
+    <t>SET MEJA KURSI ROTAN BULAT</t>
+  </si>
+  <si>
+    <t>SOFA</t>
+  </si>
+  <si>
+    <t>TABUNG GAS 12KG</t>
+  </si>
+  <si>
+    <t>TIMBANGAN</t>
+  </si>
+  <si>
+    <t>TIANG KAMERA</t>
+  </si>
+  <si>
+    <t>TANGGA</t>
+  </si>
+  <si>
+    <t>TRIPOD KAMERA</t>
+  </si>
+  <si>
+    <t>TRIPOD LAMPU</t>
+  </si>
+  <si>
+    <t>WHITEBOARD KECIL</t>
+  </si>
+  <si>
+    <t>WHITEBOARD STAND</t>
+  </si>
+  <si>
+    <t>RAK KAYU</t>
+  </si>
+  <si>
+    <t>MEJA BILIARD</t>
+  </si>
+  <si>
+    <t>GITAR CORT</t>
+  </si>
+  <si>
+    <t>DRUMB TANGAN</t>
+  </si>
+  <si>
+    <t>RAK MAINAN</t>
+  </si>
+  <si>
+    <t>MIC WIRELESS</t>
+  </si>
+  <si>
+    <t>MEJA HAMBALAN</t>
+  </si>
+  <si>
+    <t>KURSI HAMBALAN</t>
+  </si>
+  <si>
+    <t>MEJA BULAT KAYU</t>
+  </si>
+  <si>
+    <t>MEJA PERSEGI VIP</t>
+  </si>
+  <si>
+    <t>MEJA PERSEGI PANJANG VIP</t>
+  </si>
+  <si>
+    <t>MESIN GRINDER KOPI</t>
+  </si>
+  <si>
+    <t>MESIN KOPI ESPRESSO</t>
+  </si>
+  <si>
+    <t>MESIN SEALER CUP</t>
+  </si>
+  <si>
+    <t>MEJA DAPUR</t>
+  </si>
+  <si>
+    <t>MEJA LESEHAN</t>
+  </si>
+  <si>
+    <t>THERMOGUN</t>
+  </si>
+  <si>
+    <t>NODDLE BOILER</t>
+  </si>
+  <si>
+    <t>EXHAUST</t>
+  </si>
+  <si>
+    <t>DEEP FRYER</t>
+  </si>
+  <si>
+    <t>MEJA KASIR</t>
+  </si>
+  <si>
+    <t>TEMPAT DUDUK ROTAN DINDING</t>
+  </si>
+  <si>
+    <t>STICK BILLIARD</t>
+  </si>
+  <si>
+    <t>TROLI 3 TINGKAT</t>
+  </si>
+  <si>
+    <t>KURSI VIP</t>
+  </si>
+  <si>
+    <t>KURSI BAYI</t>
+  </si>
+  <si>
+    <t>KURSI HITAM</t>
+  </si>
+  <si>
+    <t>GALON</t>
+  </si>
+  <si>
+    <t>CASH DRAWER</t>
+  </si>
+  <si>
+    <t>KREY OUTDOOR</t>
+  </si>
+  <si>
+    <t>KURSI KAYU</t>
+  </si>
+  <si>
+    <t>KURSI KECIL PERSEGI</t>
+  </si>
+  <si>
+    <t>MEJA KAYU PERSEGI</t>
+  </si>
+  <si>
+    <t>MIXER AUDIO</t>
+  </si>
+  <si>
+    <t>MEJA KONSUMEN COLORADO + CHAIR BROWN</t>
+  </si>
+  <si>
+    <t>TENDA</t>
+  </si>
+  <si>
+    <t>BOR BATERAI</t>
+  </si>
+  <si>
+    <t>KUNCI PAS SET 8</t>
+  </si>
+  <si>
+    <t>SOUND SYSTEM PORTABLE</t>
+  </si>
+  <si>
+    <t>KASUR LIPAT</t>
+  </si>
+  <si>
+    <t>RAK DISPENSER 2 SUSUN</t>
+  </si>
+  <si>
+    <t>OBENG TEKIRO</t>
+  </si>
+  <si>
+    <t>KUNCI SOK Y</t>
+  </si>
+  <si>
+    <t>BLDC ALAT CEK KELISTRIKAN SEPEDA</t>
+  </si>
+  <si>
+    <t>AVOMETER</t>
+  </si>
+  <si>
+    <t>KUNCI L 1 SET</t>
+  </si>
+  <si>
+    <t>SOLDER</t>
+  </si>
+  <si>
+    <t>POMPA</t>
+  </si>
+  <si>
+    <t>LEMARI DISPLAY</t>
+  </si>
+  <si>
+    <t>MEJA TULIS 1/2 BIRO UK 120</t>
+  </si>
+  <si>
+    <t>RAMBU AKRELIK</t>
+  </si>
+  <si>
+    <t>SIGNPOLE</t>
+  </si>
+  <si>
+    <t>MIKROTIK RB951</t>
+  </si>
+  <si>
+    <t>MIKROTIK RB3011UI</t>
+  </si>
+  <si>
+    <t>UPS PROLINK 1200VA</t>
+  </si>
+  <si>
+    <t>POWER SUPPLY 500 WATT</t>
+  </si>
+  <si>
+    <t>RAM LAPTOP 4 GB</t>
+  </si>
+  <si>
+    <t>RAM LAPTOP 8 GB</t>
+  </si>
+  <si>
+    <t>SSD 250 GB</t>
+  </si>
+  <si>
+    <t>SSD 128 GB</t>
+  </si>
+  <si>
+    <t>DDR4 4 GB</t>
+  </si>
+  <si>
+    <t>VGA CARD 1 GB 64 BIT</t>
+  </si>
+  <si>
+    <t>STABILIZER MATSUNAGA</t>
+  </si>
+  <si>
+    <t>MODERN SIMBOX SERVER</t>
+  </si>
+  <si>
+    <t>PSU CCTV 20A BOX</t>
+  </si>
+  <si>
+    <t>PSU CCTV 20A JARING/FAN</t>
+  </si>
+  <si>
+    <t>HUB 5 PORT TP-LINK</t>
+  </si>
+  <si>
+    <t>UPS 600/650 VA</t>
+  </si>
+  <si>
+    <t>AC</t>
+  </si>
+  <si>
+    <t>AIR PURIFIER</t>
+  </si>
+  <si>
+    <t>ALAT FOGGING</t>
+  </si>
+  <si>
+    <t>AMPLIFIER</t>
+  </si>
+  <si>
+    <t>BLENDER</t>
+  </si>
+  <si>
+    <t>BRANKAS</t>
+  </si>
+  <si>
+    <t>DISPENSER</t>
+  </si>
+  <si>
+    <t>FIGURA</t>
+  </si>
+  <si>
+    <t>FREEZER</t>
+  </si>
+  <si>
+    <t>GENSET</t>
+  </si>
+  <si>
+    <t>INSECT KILLER</t>
+  </si>
+  <si>
+    <t>KIPAS ANGIN</t>
+  </si>
+  <si>
+    <t>KIPAS DINDING</t>
+  </si>
+  <si>
+    <t>KOMPOR</t>
+  </si>
+  <si>
+    <t>KULKAS</t>
+  </si>
+  <si>
+    <t>LED 24</t>
+  </si>
+  <si>
+    <t>LED 32</t>
+  </si>
+  <si>
+    <t>LED 50</t>
+  </si>
+  <si>
+    <t>MICROWAVE</t>
+  </si>
+  <si>
+    <t>MIC</t>
+  </si>
+  <si>
+    <t>MONEY DETECTOR</t>
+  </si>
+  <si>
+    <t>MONITOR</t>
+  </si>
+  <si>
+    <t>SEALER</t>
+  </si>
+  <si>
+    <t>SPEAKER</t>
+  </si>
+  <si>
+    <t>TIMBANGAN DIGITAL</t>
+  </si>
+  <si>
+    <t>TROLI BARANG</t>
+  </si>
+  <si>
+    <t>MOBIL</t>
+  </si>
+  <si>
+    <t>MOTOR</t>
+  </si>
+  <si>
+    <t>RICE COOKER</t>
+  </si>
+  <si>
+    <t>CHILLER</t>
+  </si>
+  <si>
+    <t>HEADSET</t>
+  </si>
+  <si>
+    <t>KAMERA CCTV OUTDOOR 2MP</t>
+  </si>
+  <si>
+    <t>KAMERA CCTV INDOOR 2MP</t>
+  </si>
+  <si>
+    <t>PC 1 SET</t>
+  </si>
+  <si>
+    <t>PRINTER</t>
+  </si>
+  <si>
+    <t>ROUTER WIFI</t>
+  </si>
+  <si>
+    <t>SCANNER BARCODE</t>
+  </si>
+  <si>
+    <t>SCANNER DOKUMEN</t>
+  </si>
+  <si>
+    <t>TABLET</t>
+  </si>
+  <si>
+    <t>HUB 16PORT</t>
+  </si>
+  <si>
+    <t>HUB 8PORT</t>
+  </si>
+  <si>
+    <t>DVR CCTV 16 CHANEL</t>
+  </si>
+  <si>
+    <t>DVR CCTV 32 CHANEL</t>
+  </si>
+  <si>
+    <t>HUB 24PORT</t>
+  </si>
+  <si>
+    <t>DVR 4 CHANEL</t>
+  </si>
+  <si>
+    <t>DVR 8 CHANEL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -373,14 +922,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="2"/>
+    <cellStyle name="Normal 3" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
@@ -682,13 +1235,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F94"/>
+  <dimension ref="A1:F273"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="B94" sqref="B94"/>
+    <sheetView tabSelected="1" topLeftCell="A246" zoomScale="81" workbookViewId="0">
+      <selection activeCell="B264" sqref="B264"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="47.42578125" customWidth="1"/>
+    <col min="2" max="2" width="35.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -718,7 +1275,7 @@
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>111</v>
       </c>
       <c r="D2">
         <v>150000</v>
@@ -726,13 +1283,13 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
         <v>9</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
       </c>
       <c r="D3">
         <v>35000</v>
@@ -740,13 +1297,13 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D4">
         <v>20000</v>
@@ -754,13 +1311,13 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D5">
         <v>20000</v>
@@ -768,13 +1325,13 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>8</v>
+        <v>111</v>
       </c>
       <c r="D6">
         <v>30000</v>
@@ -782,13 +1339,13 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B7" t="s">
         <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>8</v>
+        <v>111</v>
       </c>
       <c r="D7">
         <v>30000</v>
@@ -796,13 +1353,13 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B8" t="s">
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>8</v>
+        <v>111</v>
       </c>
       <c r="D8">
         <v>6000</v>
@@ -810,13 +1367,13 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B9" t="s">
         <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>8</v>
+        <v>111</v>
       </c>
       <c r="D9">
         <v>6000</v>
@@ -824,13 +1381,13 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B10" t="s">
         <v>7</v>
       </c>
       <c r="C10" t="s">
-        <v>8</v>
+        <v>111</v>
       </c>
       <c r="D10">
         <v>6000</v>
@@ -838,13 +1395,13 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B11" t="s">
         <v>7</v>
       </c>
       <c r="C11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D11">
         <v>6000</v>
@@ -852,13 +1409,13 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B12" t="s">
         <v>7</v>
       </c>
       <c r="C12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D12">
         <v>6000</v>
@@ -866,13 +1423,13 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B13" t="s">
         <v>7</v>
       </c>
       <c r="C13" t="s">
-        <v>8</v>
+        <v>111</v>
       </c>
       <c r="D13">
         <v>6000</v>
@@ -880,13 +1437,13 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B14" t="s">
         <v>7</v>
       </c>
       <c r="C14" t="s">
-        <v>8</v>
+        <v>111</v>
       </c>
       <c r="D14">
         <v>18000</v>
@@ -894,13 +1451,13 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B15" t="s">
         <v>7</v>
       </c>
       <c r="C15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D15">
         <v>20000</v>
@@ -908,13 +1465,13 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B16" t="s">
         <v>7</v>
       </c>
       <c r="C16" t="s">
-        <v>8</v>
+        <v>111</v>
       </c>
       <c r="D16">
         <v>140000</v>
@@ -922,13 +1479,13 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B17" t="s">
         <v>7</v>
       </c>
       <c r="C17" t="s">
-        <v>8</v>
+        <v>111</v>
       </c>
       <c r="D17">
         <v>5000</v>
@@ -936,13 +1493,13 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B18" t="s">
         <v>7</v>
       </c>
       <c r="C18" t="s">
-        <v>8</v>
+        <v>111</v>
       </c>
       <c r="D18">
         <v>30000</v>
@@ -950,13 +1507,13 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B19" t="s">
         <v>7</v>
       </c>
       <c r="C19" t="s">
-        <v>8</v>
+        <v>111</v>
       </c>
       <c r="D19">
         <v>25000</v>
@@ -964,13 +1521,13 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B20" t="s">
         <v>7</v>
       </c>
       <c r="C20" t="s">
-        <v>8</v>
+        <v>111</v>
       </c>
       <c r="D20">
         <v>8000</v>
@@ -978,13 +1535,13 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B21" t="s">
         <v>7</v>
       </c>
       <c r="C21" t="s">
-        <v>8</v>
+        <v>111</v>
       </c>
       <c r="D21">
         <v>20000</v>
@@ -992,13 +1549,13 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B22" t="s">
         <v>7</v>
       </c>
       <c r="C22" t="s">
-        <v>8</v>
+        <v>111</v>
       </c>
       <c r="D22">
         <v>4000</v>
@@ -1006,13 +1563,13 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B23" t="s">
         <v>7</v>
       </c>
       <c r="C23" t="s">
-        <v>8</v>
+        <v>111</v>
       </c>
       <c r="D23">
         <v>50000</v>
@@ -1020,13 +1577,13 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B24" t="s">
         <v>7</v>
       </c>
       <c r="C24" t="s">
-        <v>8</v>
+        <v>111</v>
       </c>
       <c r="D24">
         <v>20000</v>
@@ -1034,13 +1591,13 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B25" t="s">
         <v>7</v>
       </c>
       <c r="C25" t="s">
-        <v>8</v>
+        <v>111</v>
       </c>
       <c r="D25">
         <v>5000</v>
@@ -1048,13 +1605,13 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>32</v>
+      </c>
+      <c r="B26" t="s">
+        <v>7</v>
+      </c>
+      <c r="C26" t="s">
         <v>33</v>
-      </c>
-      <c r="B26" t="s">
-        <v>7</v>
-      </c>
-      <c r="C26" t="s">
-        <v>34</v>
       </c>
       <c r="D26">
         <v>10000</v>
@@ -1062,13 +1619,13 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B27" t="s">
         <v>7</v>
       </c>
       <c r="C27" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D27">
         <v>7000</v>
@@ -1076,13 +1633,13 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B28" t="s">
         <v>7</v>
       </c>
       <c r="C28" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D28">
         <v>5000</v>
@@ -1090,13 +1647,13 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B29" t="s">
         <v>7</v>
       </c>
       <c r="C29" t="s">
-        <v>8</v>
+        <v>111</v>
       </c>
       <c r="D29">
         <v>5000</v>
@@ -1104,13 +1661,13 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B30" t="s">
         <v>7</v>
       </c>
       <c r="C30" t="s">
-        <v>8</v>
+        <v>111</v>
       </c>
       <c r="D30">
         <v>7000</v>
@@ -1118,13 +1675,13 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B31" t="s">
         <v>7</v>
       </c>
       <c r="C31" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D31">
         <v>7000</v>
@@ -1132,13 +1689,13 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>39</v>
+      </c>
+      <c r="B32" t="s">
+        <v>7</v>
+      </c>
+      <c r="C32" t="s">
         <v>40</v>
-      </c>
-      <c r="B32" t="s">
-        <v>7</v>
-      </c>
-      <c r="C32" t="s">
-        <v>41</v>
       </c>
       <c r="D32">
         <v>5000</v>
@@ -1146,13 +1703,13 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B33" t="s">
         <v>7</v>
       </c>
       <c r="C33" t="s">
-        <v>8</v>
+        <v>111</v>
       </c>
       <c r="D33">
         <v>6000</v>
@@ -1160,13 +1717,13 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B34" t="s">
         <v>7</v>
       </c>
       <c r="C34" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D34">
         <v>2000</v>
@@ -1174,13 +1731,13 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B35" t="s">
         <v>7</v>
       </c>
       <c r="C35" t="s">
-        <v>8</v>
+        <v>111</v>
       </c>
       <c r="D35">
         <v>32000</v>
@@ -1188,13 +1745,13 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B36" t="s">
         <v>7</v>
       </c>
       <c r="C36" t="s">
-        <v>8</v>
+        <v>111</v>
       </c>
       <c r="D36">
         <v>30000</v>
@@ -1202,13 +1759,13 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B37" t="s">
         <v>7</v>
       </c>
       <c r="C37" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D37">
         <v>7000</v>
@@ -1216,13 +1773,13 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
+        <v>46</v>
+      </c>
+      <c r="B38" t="s">
+        <v>7</v>
+      </c>
+      <c r="C38" t="s">
         <v>47</v>
-      </c>
-      <c r="B38" t="s">
-        <v>7</v>
-      </c>
-      <c r="C38" t="s">
-        <v>48</v>
       </c>
       <c r="D38">
         <v>500000</v>
@@ -1230,13 +1787,13 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
+        <v>48</v>
+      </c>
+      <c r="B39" t="s">
+        <v>7</v>
+      </c>
+      <c r="C39" t="s">
         <v>49</v>
-      </c>
-      <c r="B39" t="s">
-        <v>7</v>
-      </c>
-      <c r="C39" t="s">
-        <v>50</v>
       </c>
       <c r="D39">
         <v>40000</v>
@@ -1244,13 +1801,13 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B40" t="s">
         <v>7</v>
       </c>
       <c r="C40" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D40">
         <v>40000</v>
@@ -1258,13 +1815,13 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B41" t="s">
         <v>7</v>
       </c>
       <c r="C41" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D41">
         <v>30000</v>
@@ -1272,13 +1829,13 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B42" t="s">
         <v>7</v>
       </c>
       <c r="C42" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D42">
         <v>400000</v>
@@ -1286,13 +1843,13 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B43" t="s">
         <v>7</v>
       </c>
       <c r="C43" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D43">
         <v>50000</v>
@@ -1300,13 +1857,13 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B44" t="s">
         <v>7</v>
       </c>
       <c r="C44" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D44">
         <v>8000</v>
@@ -1314,13 +1871,13 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B45" t="s">
         <v>7</v>
       </c>
       <c r="C45" t="s">
-        <v>8</v>
+        <v>111</v>
       </c>
       <c r="D45">
         <v>4000</v>
@@ -1328,13 +1885,13 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B46" t="s">
         <v>7</v>
       </c>
       <c r="C46" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D46">
         <v>8000</v>
@@ -1342,13 +1899,13 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B47" t="s">
         <v>7</v>
       </c>
       <c r="C47" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D47">
         <v>8000</v>
@@ -1356,24 +1913,24 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B48" t="s">
         <v>7</v>
       </c>
       <c r="C48" t="s">
-        <v>8</v>
+        <v>111</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B49" t="s">
         <v>7</v>
       </c>
       <c r="C49" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D49">
         <v>12000</v>
@@ -1381,13 +1938,13 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B50" t="s">
         <v>7</v>
       </c>
       <c r="C50" t="s">
-        <v>8</v>
+        <v>111</v>
       </c>
       <c r="D50">
         <v>10000</v>
@@ -1395,13 +1952,13 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B51" t="s">
         <v>7</v>
       </c>
       <c r="C51" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D51">
         <v>40000</v>
@@ -1409,13 +1966,13 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B52" t="s">
         <v>7</v>
       </c>
       <c r="C52" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D52">
         <v>25000</v>
@@ -1423,13 +1980,13 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B53" t="s">
         <v>7</v>
       </c>
       <c r="C53" t="s">
-        <v>8</v>
+        <v>111</v>
       </c>
       <c r="D53">
         <v>10000</v>
@@ -1437,13 +1994,13 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B54" t="s">
         <v>7</v>
       </c>
       <c r="C54" t="s">
-        <v>8</v>
+        <v>111</v>
       </c>
       <c r="D54">
         <v>10000</v>
@@ -1451,13 +2008,13 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B55" t="s">
         <v>7</v>
       </c>
       <c r="C55" t="s">
-        <v>8</v>
+        <v>111</v>
       </c>
       <c r="D55">
         <v>40000</v>
@@ -1465,13 +2022,13 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B56" t="s">
         <v>7</v>
       </c>
       <c r="C56" t="s">
-        <v>8</v>
+        <v>111</v>
       </c>
       <c r="D56">
         <v>3000</v>
@@ -1479,13 +2036,13 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B57" t="s">
         <v>7</v>
       </c>
       <c r="C57" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D57">
         <v>7000</v>
@@ -1493,13 +2050,13 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B58" t="s">
         <v>7</v>
       </c>
       <c r="C58" t="s">
-        <v>8</v>
+        <v>111</v>
       </c>
       <c r="D58">
         <v>8000</v>
@@ -1507,13 +2064,13 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B59" t="s">
         <v>7</v>
       </c>
       <c r="C59" t="s">
-        <v>8</v>
+        <v>111</v>
       </c>
       <c r="D59">
         <v>10000</v>
@@ -1521,13 +2078,13 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B60" t="s">
         <v>7</v>
       </c>
       <c r="C60" t="s">
-        <v>8</v>
+        <v>111</v>
       </c>
       <c r="D60">
         <v>5000</v>
@@ -1535,13 +2092,13 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B61" t="s">
         <v>7</v>
       </c>
       <c r="C61" t="s">
-        <v>8</v>
+        <v>111</v>
       </c>
       <c r="D61">
         <v>15000</v>
@@ -1549,13 +2106,13 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B62" t="s">
         <v>7</v>
       </c>
       <c r="C62" t="s">
-        <v>8</v>
+        <v>111</v>
       </c>
       <c r="D62">
         <v>30000</v>
@@ -1563,13 +2120,13 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B63" t="s">
         <v>7</v>
       </c>
       <c r="C63" t="s">
-        <v>8</v>
+        <v>111</v>
       </c>
       <c r="D63">
         <v>50000</v>
@@ -1577,35 +2134,35 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B64" t="s">
         <v>7</v>
       </c>
       <c r="C64" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B65" t="s">
         <v>7</v>
       </c>
       <c r="C65" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B66" t="s">
         <v>7</v>
       </c>
       <c r="C66" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D66">
         <v>5000</v>
@@ -1613,13 +2170,13 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B67" t="s">
         <v>7</v>
       </c>
       <c r="C67" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D67">
         <v>16000</v>
@@ -1627,13 +2184,13 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B68" t="s">
         <v>7</v>
       </c>
       <c r="C68" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D68">
         <v>18000</v>
@@ -1641,13 +2198,13 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B69" t="s">
         <v>7</v>
       </c>
       <c r="C69" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D69">
         <v>20000</v>
@@ -1655,13 +2212,13 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B70" t="s">
         <v>7</v>
       </c>
       <c r="C70" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D70">
         <v>33000</v>
@@ -1669,13 +2226,13 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B71" t="s">
         <v>7</v>
       </c>
       <c r="C71" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D71">
         <v>33000</v>
@@ -1683,13 +2240,13 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B72" t="s">
         <v>7</v>
       </c>
       <c r="C72" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D72">
         <v>37000</v>
@@ -1697,13 +2254,13 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B73" t="s">
         <v>7</v>
       </c>
       <c r="C73" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D73">
         <v>27000</v>
@@ -1711,13 +2268,13 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B74" t="s">
         <v>7</v>
       </c>
       <c r="C74" t="s">
-        <v>8</v>
+        <v>111</v>
       </c>
       <c r="D74">
         <v>2000</v>
@@ -1725,13 +2282,13 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B75" t="s">
         <v>7</v>
       </c>
       <c r="C75" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D75">
         <v>7000</v>
@@ -1739,13 +2296,13 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B76" t="s">
         <v>7</v>
       </c>
       <c r="C76" t="s">
-        <v>8</v>
+        <v>111</v>
       </c>
       <c r="D76">
         <v>5000</v>
@@ -1753,13 +2310,13 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B77" t="s">
         <v>7</v>
       </c>
       <c r="C77" t="s">
-        <v>8</v>
+        <v>111</v>
       </c>
       <c r="D77">
         <v>100000</v>
@@ -1767,234 +2324,2194 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B78" t="s">
         <v>7</v>
       </c>
       <c r="C78" t="s">
-        <v>8</v>
+        <v>111</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B79" t="s">
         <v>7</v>
       </c>
       <c r="C79" t="s">
-        <v>8</v>
+        <v>111</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B80" t="s">
         <v>7</v>
       </c>
       <c r="C80" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D80">
         <v>3000</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B81" t="s">
         <v>7</v>
       </c>
       <c r="C81" t="s">
-        <v>8</v>
+        <v>111</v>
       </c>
       <c r="D81">
         <v>7000</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B82" t="s">
         <v>7</v>
       </c>
       <c r="C82" t="s">
-        <v>8</v>
+        <v>111</v>
       </c>
       <c r="D82">
         <v>7000</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B83" t="s">
         <v>7</v>
       </c>
       <c r="C83" t="s">
-        <v>8</v>
+        <v>111</v>
       </c>
       <c r="D83">
         <v>5000</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B84" t="s">
         <v>7</v>
       </c>
       <c r="C84" t="s">
-        <v>8</v>
+        <v>111</v>
       </c>
       <c r="D84">
         <v>5000</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B85" t="s">
         <v>7</v>
       </c>
       <c r="C85" t="s">
-        <v>8</v>
+        <v>111</v>
       </c>
       <c r="D85">
         <v>10000</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B86" t="s">
         <v>7</v>
       </c>
       <c r="C86" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D86">
         <v>10000</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
+        <v>97</v>
+      </c>
+      <c r="B87" t="s">
+        <v>7</v>
+      </c>
+      <c r="C87" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
         <v>98</v>
       </c>
-      <c r="B87" t="s">
-        <v>7</v>
-      </c>
-      <c r="C87" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
+      <c r="B88" t="s">
+        <v>7</v>
+      </c>
+      <c r="C88" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
         <v>99</v>
       </c>
-      <c r="B88" t="s">
-        <v>7</v>
-      </c>
-      <c r="C88" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
-        <v>100</v>
-      </c>
       <c r="B89" t="s">
         <v>7</v>
       </c>
       <c r="C89" t="s">
-        <v>8</v>
+        <v>111</v>
       </c>
       <c r="D89">
         <v>30000</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B90" t="s">
         <v>7</v>
       </c>
       <c r="C90" t="s">
-        <v>8</v>
+        <v>111</v>
       </c>
       <c r="D90">
         <v>20000</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B91" t="s">
         <v>7</v>
       </c>
       <c r="C91" t="s">
-        <v>8</v>
+        <v>111</v>
       </c>
       <c r="D91">
         <v>25000</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B92" t="s">
         <v>7</v>
       </c>
       <c r="C92" t="s">
-        <v>8</v>
+        <v>111</v>
       </c>
       <c r="D92">
         <v>5000</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B93" t="s">
         <v>7</v>
       </c>
       <c r="C93" t="s">
-        <v>8</v>
+        <v>111</v>
       </c>
       <c r="D93">
         <v>10000</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
+        <v>240</v>
+      </c>
+      <c r="B94" t="s">
+        <v>104</v>
+      </c>
+      <c r="C94" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>241</v>
+      </c>
+      <c r="B95" t="s">
+        <v>104</v>
+      </c>
+      <c r="C95" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>242</v>
+      </c>
+      <c r="B96" t="s">
+        <v>104</v>
+      </c>
+      <c r="C96" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>243</v>
+      </c>
+      <c r="B97" t="s">
+        <v>104</v>
+      </c>
+      <c r="C97" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>112</v>
+      </c>
+      <c r="B98" t="s">
+        <v>104</v>
+      </c>
+      <c r="C98" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>113</v>
+      </c>
+      <c r="B99" t="s">
+        <v>104</v>
+      </c>
+      <c r="C99" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>244</v>
+      </c>
+      <c r="B100" t="s">
+        <v>104</v>
+      </c>
+      <c r="C100" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>114</v>
+      </c>
+      <c r="B101" t="s">
+        <v>104</v>
+      </c>
+      <c r="C101" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>245</v>
+      </c>
+      <c r="B102" t="s">
+        <v>104</v>
+      </c>
+      <c r="C102" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>115</v>
+      </c>
+      <c r="B103" t="s">
+        <v>104</v>
+      </c>
+      <c r="C103" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>246</v>
+      </c>
+      <c r="B104" t="s">
+        <v>104</v>
+      </c>
+      <c r="C104" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>247</v>
+      </c>
+      <c r="B105" t="s">
+        <v>104</v>
+      </c>
+      <c r="C105" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>116</v>
+      </c>
+      <c r="B106" t="s">
+        <v>104</v>
+      </c>
+      <c r="C106" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>117</v>
+      </c>
+      <c r="B107" t="s">
+        <v>104</v>
+      </c>
+      <c r="C107" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>248</v>
+      </c>
+      <c r="B108" t="s">
+        <v>104</v>
+      </c>
+      <c r="C108" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>249</v>
+      </c>
+      <c r="B109" t="s">
+        <v>104</v>
+      </c>
+      <c r="C109" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>118</v>
+      </c>
+      <c r="B110" t="s">
+        <v>104</v>
+      </c>
+      <c r="C110" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>119</v>
+      </c>
+      <c r="B111" t="s">
+        <v>104</v>
+      </c>
+      <c r="C111" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>120</v>
+      </c>
+      <c r="B112" t="s">
+        <v>104</v>
+      </c>
+      <c r="C112" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>121</v>
+      </c>
+      <c r="B113" t="s">
+        <v>104</v>
+      </c>
+      <c r="C113" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>250</v>
+      </c>
+      <c r="B114" t="s">
+        <v>104</v>
+      </c>
+      <c r="C114" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>122</v>
+      </c>
+      <c r="B115" t="s">
+        <v>104</v>
+      </c>
+      <c r="C115" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>123</v>
+      </c>
+      <c r="B116" t="s">
+        <v>104</v>
+      </c>
+      <c r="C116" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>251</v>
+      </c>
+      <c r="B117" t="s">
+        <v>104</v>
+      </c>
+      <c r="C117" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>252</v>
+      </c>
+      <c r="B118" t="s">
+        <v>104</v>
+      </c>
+      <c r="C118" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>124</v>
+      </c>
+      <c r="B119" t="s">
+        <v>104</v>
+      </c>
+      <c r="C119" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>125</v>
+      </c>
+      <c r="B120" t="s">
+        <v>104</v>
+      </c>
+      <c r="C120" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>253</v>
+      </c>
+      <c r="B121" t="s">
+        <v>104</v>
+      </c>
+      <c r="C121" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>254</v>
+      </c>
+      <c r="B122" t="s">
+        <v>104</v>
+      </c>
+      <c r="C122" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>126</v>
+      </c>
+      <c r="B123" t="s">
+        <v>104</v>
+      </c>
+      <c r="C123" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
         <v>105</v>
       </c>
-      <c r="B94" t="s">
+      <c r="B124" t="s">
+        <v>104</v>
+      </c>
+      <c r="C124" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>127</v>
+      </c>
+      <c r="B125" t="s">
+        <v>104</v>
+      </c>
+      <c r="C125" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>128</v>
+      </c>
+      <c r="B126" t="s">
+        <v>104</v>
+      </c>
+      <c r="C126" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>129</v>
+      </c>
+      <c r="B127" t="s">
+        <v>104</v>
+      </c>
+      <c r="C127" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>130</v>
+      </c>
+      <c r="B128" t="s">
+        <v>104</v>
+      </c>
+      <c r="C128" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>106</v>
+      </c>
+      <c r="B129" t="s">
+        <v>104</v>
+      </c>
+      <c r="C129" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>131</v>
+      </c>
+      <c r="B130" t="s">
+        <v>104</v>
+      </c>
+      <c r="C130" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>132</v>
+      </c>
+      <c r="B131" t="s">
+        <v>104</v>
+      </c>
+      <c r="C131" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
         <v>107</v>
       </c>
-      <c r="C94" t="s">
-        <v>8</v>
-      </c>
-      <c r="D94">
-        <v>7000000</v>
-      </c>
-      <c r="E94" t="s">
-        <v>106</v>
-      </c>
-      <c r="F94">
-        <v>1</v>
+      <c r="B132" t="s">
+        <v>104</v>
+      </c>
+      <c r="C132" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>133</v>
+      </c>
+      <c r="B133" t="s">
+        <v>104</v>
+      </c>
+      <c r="C133" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>134</v>
+      </c>
+      <c r="B134" t="s">
+        <v>104</v>
+      </c>
+      <c r="C134" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>255</v>
+      </c>
+      <c r="B135" t="s">
+        <v>104</v>
+      </c>
+      <c r="C135" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>256</v>
+      </c>
+      <c r="B136" t="s">
+        <v>104</v>
+      </c>
+      <c r="C136" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>257</v>
+      </c>
+      <c r="B137" t="s">
+        <v>104</v>
+      </c>
+      <c r="C137" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>135</v>
+      </c>
+      <c r="B138" t="s">
+        <v>104</v>
+      </c>
+      <c r="C138" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>136</v>
+      </c>
+      <c r="B139" t="s">
+        <v>104</v>
+      </c>
+      <c r="C139" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
+        <v>137</v>
+      </c>
+      <c r="B140" t="s">
+        <v>104</v>
+      </c>
+      <c r="C140" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
+        <v>108</v>
+      </c>
+      <c r="B141" t="s">
+        <v>104</v>
+      </c>
+      <c r="C141" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
+        <v>138</v>
+      </c>
+      <c r="B142" t="s">
+        <v>104</v>
+      </c>
+      <c r="C142" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>139</v>
+      </c>
+      <c r="B143" t="s">
+        <v>104</v>
+      </c>
+      <c r="C143" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
+        <v>140</v>
+      </c>
+      <c r="B144" t="s">
+        <v>104</v>
+      </c>
+      <c r="C144" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
+        <v>141</v>
+      </c>
+      <c r="B145" t="s">
+        <v>104</v>
+      </c>
+      <c r="C145" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>142</v>
+      </c>
+      <c r="B146" t="s">
+        <v>104</v>
+      </c>
+      <c r="C146" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
+        <v>143</v>
+      </c>
+      <c r="B147" t="s">
+        <v>104</v>
+      </c>
+      <c r="C147" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
+        <v>109</v>
+      </c>
+      <c r="B148" t="s">
+        <v>104</v>
+      </c>
+      <c r="C148" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>144</v>
+      </c>
+      <c r="B149" t="s">
+        <v>104</v>
+      </c>
+      <c r="C149" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
+        <v>110</v>
+      </c>
+      <c r="B150" t="s">
+        <v>104</v>
+      </c>
+      <c r="C150" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
+        <v>145</v>
+      </c>
+      <c r="B151" t="s">
+        <v>104</v>
+      </c>
+      <c r="C151" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
+        <v>146</v>
+      </c>
+      <c r="B152" t="s">
+        <v>104</v>
+      </c>
+      <c r="C152" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
+        <v>147</v>
+      </c>
+      <c r="B153" t="s">
+        <v>104</v>
+      </c>
+      <c r="C153" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
+        <v>148</v>
+      </c>
+      <c r="B154" t="s">
+        <v>104</v>
+      </c>
+      <c r="C154" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>149</v>
+      </c>
+      <c r="B155" t="s">
+        <v>104</v>
+      </c>
+      <c r="C155" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
+        <v>150</v>
+      </c>
+      <c r="B156" t="s">
+        <v>104</v>
+      </c>
+      <c r="C156" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
+        <v>151</v>
+      </c>
+      <c r="B157" t="s">
+        <v>104</v>
+      </c>
+      <c r="C157" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
+        <v>152</v>
+      </c>
+      <c r="B158" t="s">
+        <v>104</v>
+      </c>
+      <c r="C158" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
+        <v>153</v>
+      </c>
+      <c r="B159" t="s">
+        <v>104</v>
+      </c>
+      <c r="C159" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
+        <v>154</v>
+      </c>
+      <c r="B160" t="s">
+        <v>104</v>
+      </c>
+      <c r="C160" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
+        <v>259</v>
+      </c>
+      <c r="B161" t="s">
+        <v>104</v>
+      </c>
+      <c r="C161" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A162" t="s">
+        <v>258</v>
+      </c>
+      <c r="B162" t="s">
+        <v>104</v>
+      </c>
+      <c r="C162" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
+        <v>260</v>
+      </c>
+      <c r="B163" t="s">
+        <v>104</v>
+      </c>
+      <c r="C163" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
+        <v>261</v>
+      </c>
+      <c r="B164" t="s">
+        <v>104</v>
+      </c>
+      <c r="C164" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
+        <v>155</v>
+      </c>
+      <c r="B165" t="s">
+        <v>104</v>
+      </c>
+      <c r="C165" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A166" t="s">
+        <v>156</v>
+      </c>
+      <c r="B166" t="s">
+        <v>104</v>
+      </c>
+      <c r="C166" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A167" t="s">
+        <v>157</v>
+      </c>
+      <c r="B167" t="s">
+        <v>104</v>
+      </c>
+      <c r="C167" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A168" t="s">
+        <v>158</v>
+      </c>
+      <c r="B168" t="s">
+        <v>104</v>
+      </c>
+      <c r="C168" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A169" t="s">
+        <v>159</v>
+      </c>
+      <c r="B169" t="s">
+        <v>104</v>
+      </c>
+      <c r="C169" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A170" t="s">
+        <v>262</v>
+      </c>
+      <c r="B170" t="s">
+        <v>104</v>
+      </c>
+      <c r="C170" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A171" t="s">
+        <v>160</v>
+      </c>
+      <c r="B171" t="s">
+        <v>104</v>
+      </c>
+      <c r="C171" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A172" t="s">
+        <v>161</v>
+      </c>
+      <c r="B172" t="s">
+        <v>104</v>
+      </c>
+      <c r="C172" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A173" t="s">
+        <v>162</v>
+      </c>
+      <c r="B173" t="s">
+        <v>104</v>
+      </c>
+      <c r="C173" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A174" t="s">
+        <v>163</v>
+      </c>
+      <c r="B174" t="s">
+        <v>104</v>
+      </c>
+      <c r="C174" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A175" t="s">
+        <v>263</v>
+      </c>
+      <c r="B175" t="s">
+        <v>104</v>
+      </c>
+      <c r="C175" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A176" t="s">
+        <v>164</v>
+      </c>
+      <c r="B176" t="s">
+        <v>104</v>
+      </c>
+      <c r="C176" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A177" t="s">
+        <v>165</v>
+      </c>
+      <c r="B177" t="s">
+        <v>104</v>
+      </c>
+      <c r="C177" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A178" t="s">
+        <v>166</v>
+      </c>
+      <c r="B178" t="s">
+        <v>104</v>
+      </c>
+      <c r="C178" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A179" t="s">
+        <v>167</v>
+      </c>
+      <c r="B179" t="s">
+        <v>104</v>
+      </c>
+      <c r="C179" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A180" t="s">
+        <v>264</v>
+      </c>
+      <c r="B180" t="s">
+        <v>104</v>
+      </c>
+      <c r="C180" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A181" t="s">
+        <v>168</v>
+      </c>
+      <c r="B181" t="s">
+        <v>104</v>
+      </c>
+      <c r="C181" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A182" t="s">
+        <v>169</v>
+      </c>
+      <c r="B182" t="s">
+        <v>104</v>
+      </c>
+      <c r="C182" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A183" t="s">
+        <v>265</v>
+      </c>
+      <c r="B183" t="s">
+        <v>104</v>
+      </c>
+      <c r="C183" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A184" t="s">
+        <v>170</v>
+      </c>
+      <c r="B184" t="s">
+        <v>104</v>
+      </c>
+      <c r="C184" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A185" t="s">
+        <v>171</v>
+      </c>
+      <c r="B185" t="s">
+        <v>104</v>
+      </c>
+      <c r="C185" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A186" t="s">
+        <v>172</v>
+      </c>
+      <c r="B186" t="s">
+        <v>104</v>
+      </c>
+      <c r="C186" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A187" t="s">
+        <v>266</v>
+      </c>
+      <c r="B187" t="s">
+        <v>104</v>
+      </c>
+      <c r="C187" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A188" t="s">
+        <v>267</v>
+      </c>
+      <c r="B188" t="s">
+        <v>104</v>
+      </c>
+      <c r="C188" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A189" t="s">
+        <v>173</v>
+      </c>
+      <c r="B189" t="s">
+        <v>104</v>
+      </c>
+      <c r="C189" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A190" t="s">
+        <v>174</v>
+      </c>
+      <c r="B190" t="s">
+        <v>104</v>
+      </c>
+      <c r="C190" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A191" t="s">
+        <v>175</v>
+      </c>
+      <c r="B191" t="s">
+        <v>104</v>
+      </c>
+      <c r="C191" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A192" t="s">
+        <v>176</v>
+      </c>
+      <c r="B192" t="s">
+        <v>104</v>
+      </c>
+      <c r="C192" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A193" t="s">
+        <v>177</v>
+      </c>
+      <c r="B193" t="s">
+        <v>104</v>
+      </c>
+      <c r="C193" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A194" t="s">
+        <v>178</v>
+      </c>
+      <c r="B194" t="s">
+        <v>104</v>
+      </c>
+      <c r="C194" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A195" t="s">
+        <v>179</v>
+      </c>
+      <c r="B195" t="s">
+        <v>104</v>
+      </c>
+      <c r="C195" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A196" t="s">
+        <v>180</v>
+      </c>
+      <c r="B196" t="s">
+        <v>104</v>
+      </c>
+      <c r="C196" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A197" t="s">
+        <v>181</v>
+      </c>
+      <c r="B197" t="s">
+        <v>104</v>
+      </c>
+      <c r="C197" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A198" t="s">
+        <v>182</v>
+      </c>
+      <c r="B198" t="s">
+        <v>104</v>
+      </c>
+      <c r="C198" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A199" t="s">
+        <v>183</v>
+      </c>
+      <c r="B199" t="s">
+        <v>104</v>
+      </c>
+      <c r="C199" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A200" t="s">
+        <v>184</v>
+      </c>
+      <c r="B200" t="s">
+        <v>104</v>
+      </c>
+      <c r="C200" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="201" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A201" t="s">
+        <v>185</v>
+      </c>
+      <c r="B201" t="s">
+        <v>104</v>
+      </c>
+      <c r="C201" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="202" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A202" t="s">
+        <v>186</v>
+      </c>
+      <c r="B202" t="s">
+        <v>104</v>
+      </c>
+      <c r="C202" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="203" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A203" t="s">
+        <v>187</v>
+      </c>
+      <c r="B203" t="s">
+        <v>104</v>
+      </c>
+      <c r="C203" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="204" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A204" t="s">
+        <v>268</v>
+      </c>
+      <c r="B204" t="s">
+        <v>104</v>
+      </c>
+      <c r="C204" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="205" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A205" t="s">
+        <v>188</v>
+      </c>
+      <c r="B205" t="s">
+        <v>104</v>
+      </c>
+      <c r="C205" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="206" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A206" t="s">
+        <v>189</v>
+      </c>
+      <c r="B206" t="s">
+        <v>104</v>
+      </c>
+      <c r="C206" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="207" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A207" t="s">
+        <v>190</v>
+      </c>
+      <c r="B207" t="s">
+        <v>104</v>
+      </c>
+      <c r="C207" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="208" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A208" t="s">
+        <v>269</v>
+      </c>
+      <c r="B208" t="s">
+        <v>104</v>
+      </c>
+      <c r="C208" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="209" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A209" t="s">
+        <v>191</v>
+      </c>
+      <c r="B209" t="s">
+        <v>104</v>
+      </c>
+      <c r="C209" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="210" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A210" t="s">
+        <v>192</v>
+      </c>
+      <c r="B210" t="s">
+        <v>104</v>
+      </c>
+      <c r="C210" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="211" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A211" t="s">
+        <v>193</v>
+      </c>
+      <c r="B211" t="s">
+        <v>104</v>
+      </c>
+      <c r="C211" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="212" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A212" t="s">
+        <v>194</v>
+      </c>
+      <c r="B212" t="s">
+        <v>104</v>
+      </c>
+      <c r="C212" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="213" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A213" t="s">
+        <v>195</v>
+      </c>
+      <c r="B213" t="s">
+        <v>104</v>
+      </c>
+      <c r="C213" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="214" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A214" t="s">
+        <v>196</v>
+      </c>
+      <c r="B214" t="s">
+        <v>104</v>
+      </c>
+      <c r="C214" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="215" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A215" t="s">
+        <v>197</v>
+      </c>
+      <c r="B215" t="s">
+        <v>104</v>
+      </c>
+      <c r="C215" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="216" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A216" t="s">
+        <v>198</v>
+      </c>
+      <c r="B216" t="s">
+        <v>104</v>
+      </c>
+      <c r="C216" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="217" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A217" t="s">
+        <v>199</v>
+      </c>
+      <c r="B217" t="s">
+        <v>104</v>
+      </c>
+      <c r="C217" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="218" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A218" t="s">
+        <v>200</v>
+      </c>
+      <c r="B218" t="s">
+        <v>104</v>
+      </c>
+      <c r="C218" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="219" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A219" t="s">
+        <v>201</v>
+      </c>
+      <c r="B219" t="s">
+        <v>104</v>
+      </c>
+      <c r="C219" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="220" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A220" t="s">
+        <v>202</v>
+      </c>
+      <c r="B220" t="s">
+        <v>104</v>
+      </c>
+      <c r="C220" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="221" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A221" t="s">
+        <v>203</v>
+      </c>
+      <c r="B221" t="s">
+        <v>104</v>
+      </c>
+      <c r="C221" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="222" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A222" t="s">
+        <v>204</v>
+      </c>
+      <c r="B222" t="s">
+        <v>104</v>
+      </c>
+      <c r="C222" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="223" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A223" t="s">
+        <v>205</v>
+      </c>
+      <c r="B223" t="s">
+        <v>104</v>
+      </c>
+      <c r="C223" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="224" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A224" t="s">
+        <v>206</v>
+      </c>
+      <c r="B224" t="s">
+        <v>104</v>
+      </c>
+      <c r="C224" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="225" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A225" t="s">
+        <v>207</v>
+      </c>
+      <c r="B225" t="s">
+        <v>104</v>
+      </c>
+      <c r="C225" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="226" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A226" t="s">
+        <v>208</v>
+      </c>
+      <c r="B226" t="s">
+        <v>104</v>
+      </c>
+      <c r="C226" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="227" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A227" t="s">
+        <v>209</v>
+      </c>
+      <c r="B227" t="s">
+        <v>104</v>
+      </c>
+      <c r="C227" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="228" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A228" t="s">
+        <v>210</v>
+      </c>
+      <c r="B228" t="s">
+        <v>104</v>
+      </c>
+      <c r="C228" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="229" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A229" t="s">
+        <v>211</v>
+      </c>
+      <c r="B229" t="s">
+        <v>104</v>
+      </c>
+      <c r="C229" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="230" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A230" t="s">
+        <v>212</v>
+      </c>
+      <c r="B230" t="s">
+        <v>104</v>
+      </c>
+      <c r="C230" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="231" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A231" t="s">
+        <v>213</v>
+      </c>
+      <c r="B231" t="s">
+        <v>104</v>
+      </c>
+      <c r="C231" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="232" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A232" t="s">
+        <v>214</v>
+      </c>
+      <c r="B232" t="s">
+        <v>104</v>
+      </c>
+      <c r="C232" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="233" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A233" t="s">
+        <v>215</v>
+      </c>
+      <c r="B233" t="s">
+        <v>104</v>
+      </c>
+      <c r="C233" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="234" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A234" t="s">
+        <v>216</v>
+      </c>
+      <c r="B234" t="s">
+        <v>104</v>
+      </c>
+      <c r="C234" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="235" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A235" t="s">
+        <v>217</v>
+      </c>
+      <c r="B235" t="s">
+        <v>104</v>
+      </c>
+      <c r="C235" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="236" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A236" t="s">
+        <v>218</v>
+      </c>
+      <c r="B236" t="s">
+        <v>104</v>
+      </c>
+      <c r="C236" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="237" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A237" t="s">
+        <v>219</v>
+      </c>
+      <c r="B237" t="s">
+        <v>104</v>
+      </c>
+      <c r="C237" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="238" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A238" t="s">
+        <v>220</v>
+      </c>
+      <c r="B238" t="s">
+        <v>104</v>
+      </c>
+      <c r="C238" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="239" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A239" t="s">
+        <v>221</v>
+      </c>
+      <c r="B239" t="s">
+        <v>104</v>
+      </c>
+      <c r="C239" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="240" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A240" t="s">
+        <v>222</v>
+      </c>
+      <c r="B240" t="s">
+        <v>104</v>
+      </c>
+      <c r="C240" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="241" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A241" t="s">
+        <v>223</v>
+      </c>
+      <c r="B241" t="s">
+        <v>104</v>
+      </c>
+      <c r="C241" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="242" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A242" t="s">
+        <v>224</v>
+      </c>
+      <c r="B242" t="s">
+        <v>104</v>
+      </c>
+      <c r="C242" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="243" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A243" t="s">
+        <v>270</v>
+      </c>
+      <c r="B243" t="s">
+        <v>104</v>
+      </c>
+      <c r="C243" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="244" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A244" t="s">
+        <v>282</v>
+      </c>
+      <c r="B244" t="s">
+        <v>104</v>
+      </c>
+      <c r="C244" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="245" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A245" t="s">
+        <v>281</v>
+      </c>
+      <c r="B245" t="s">
+        <v>104</v>
+      </c>
+      <c r="C245" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="246" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A246" t="s">
+        <v>280</v>
+      </c>
+      <c r="B246" t="s">
+        <v>104</v>
+      </c>
+      <c r="C246" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="247" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A247" t="s">
+        <v>279</v>
+      </c>
+      <c r="B247" t="s">
+        <v>104</v>
+      </c>
+      <c r="C247" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="248" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A248" t="s">
+        <v>271</v>
+      </c>
+      <c r="B248" t="s">
+        <v>104</v>
+      </c>
+      <c r="C248" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="249" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A249" t="s">
+        <v>272</v>
+      </c>
+      <c r="B249" t="s">
+        <v>104</v>
+      </c>
+      <c r="C249" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="250" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A250" t="s">
+        <v>273</v>
+      </c>
+      <c r="B250" t="s">
+        <v>104</v>
+      </c>
+      <c r="C250" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="251" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A251" t="s">
+        <v>274</v>
+      </c>
+      <c r="B251" t="s">
+        <v>104</v>
+      </c>
+      <c r="C251" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="252" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A252" t="s">
+        <v>275</v>
+      </c>
+      <c r="B252" t="s">
+        <v>104</v>
+      </c>
+      <c r="C252" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="253" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A253" t="s">
+        <v>276</v>
+      </c>
+      <c r="B253" t="s">
+        <v>104</v>
+      </c>
+      <c r="C253" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="254" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A254" t="s">
+        <v>277</v>
+      </c>
+      <c r="B254" t="s">
+        <v>104</v>
+      </c>
+      <c r="C254" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="255" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A255" t="s">
+        <v>283</v>
+      </c>
+      <c r="B255" t="s">
+        <v>104</v>
+      </c>
+      <c r="C255" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="256" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A256" t="s">
+        <v>225</v>
+      </c>
+      <c r="B256" t="s">
+        <v>104</v>
+      </c>
+      <c r="C256" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="257" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A257" t="s">
+        <v>226</v>
+      </c>
+      <c r="B257" t="s">
+        <v>104</v>
+      </c>
+      <c r="C257" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="258" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A258" t="s">
+        <v>278</v>
+      </c>
+      <c r="B258" t="s">
+        <v>104</v>
+      </c>
+      <c r="C258" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="259" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A259" t="s">
+        <v>227</v>
+      </c>
+      <c r="B259" t="s">
+        <v>104</v>
+      </c>
+      <c r="C259" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="260" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A260" t="s">
+        <v>228</v>
+      </c>
+      <c r="B260" t="s">
+        <v>104</v>
+      </c>
+      <c r="C260" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="261" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A261" t="s">
+        <v>229</v>
+      </c>
+      <c r="B261" t="s">
+        <v>104</v>
+      </c>
+      <c r="C261" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="262" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A262" t="s">
+        <v>230</v>
+      </c>
+      <c r="B262" t="s">
+        <v>104</v>
+      </c>
+      <c r="C262" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="263" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A263" t="s">
+        <v>231</v>
+      </c>
+      <c r="B263" t="s">
+        <v>104</v>
+      </c>
+      <c r="C263" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="264" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A264" t="s">
+        <v>232</v>
+      </c>
+      <c r="B264" t="s">
+        <v>104</v>
+      </c>
+      <c r="C264" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="265" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A265" t="s">
+        <v>233</v>
+      </c>
+      <c r="B265" t="s">
+        <v>104</v>
+      </c>
+      <c r="C265" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="266" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A266" t="s">
+        <v>234</v>
+      </c>
+      <c r="B266" t="s">
+        <v>104</v>
+      </c>
+      <c r="C266" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="267" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A267" t="s">
+        <v>235</v>
+      </c>
+      <c r="B267" t="s">
+        <v>104</v>
+      </c>
+      <c r="C267" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="268" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A268" t="s">
+        <v>285</v>
+      </c>
+      <c r="B268" t="s">
+        <v>104</v>
+      </c>
+      <c r="C268" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="269" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A269" t="s">
+        <v>284</v>
+      </c>
+      <c r="B269" t="s">
+        <v>104</v>
+      </c>
+      <c r="C269" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="270" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A270" t="s">
+        <v>236</v>
+      </c>
+      <c r="B270" t="s">
+        <v>104</v>
+      </c>
+      <c r="C270" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="271" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A271" t="s">
+        <v>237</v>
+      </c>
+      <c r="B271" t="s">
+        <v>104</v>
+      </c>
+      <c r="C271" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="272" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A272" t="s">
+        <v>238</v>
+      </c>
+      <c r="B272" t="s">
+        <v>104</v>
+      </c>
+      <c r="C272" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="273" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A273" t="s">
+        <v>239</v>
+      </c>
+      <c r="B273" t="s">
+        <v>104</v>
+      </c>
+      <c r="C273" t="s">
+        <v>111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
nambah divisi, area, 2 url
</commit_message>
<xml_diff>
--- a/storage/import/barang.xlsx
+++ b/storage/import/barang.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="822" uniqueCount="286">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="825" uniqueCount="288">
   <si>
     <t>nama_barang</t>
   </si>
@@ -877,6 +877,12 @@
   </si>
   <si>
     <t>DVR 8 CHANEL</t>
+  </si>
+  <si>
+    <t>NOTA MANUAL</t>
+  </si>
+  <si>
+    <t>NOTA</t>
   </si>
 </sst>
 </file>
@@ -1235,10 +1241,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F273"/>
+  <dimension ref="A1:F274"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="81" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="A266" zoomScale="81" workbookViewId="0">
+      <selection activeCell="B275" sqref="B275"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4514,6 +4520,17 @@
         <v>111</v>
       </c>
     </row>
+    <row r="274" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A274" t="s">
+        <v>286</v>
+      </c>
+      <c r="B274" t="s">
+        <v>287</v>
+      </c>
+      <c r="C274" t="s">
+        <v>111</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>